<commit_message>
Incluye las medidas de dispersion
</commit_message>
<xml_diff>
--- a/04/PoblacionMundial.xlsx
+++ b/04/PoblacionMundial.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="252">
   <si>
     <t>Continente</t>
   </si>
@@ -811,6 +811,24 @@
   </si>
   <si>
     <t>3er cuartil</t>
+  </si>
+  <si>
+    <t>Medidas de dispersión</t>
+  </si>
+  <si>
+    <t>Recorrido</t>
+  </si>
+  <si>
+    <t>Recorrido intercuartílico</t>
+  </si>
+  <si>
+    <t>Varianza</t>
+  </si>
+  <si>
+    <t>Desviación</t>
+  </si>
+  <si>
+    <t>Coef. Var. Pearson</t>
   </si>
 </sst>
 </file>
@@ -1313,14 +1331,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="I237" sqref="I237"/>
+    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="F231" sqref="F231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6699,13 +6719,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A226" s="10" t="s">
         <v>241</v>
       </c>
       <c r="B226" s="10"/>
-    </row>
-    <row r="227" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D226" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="E226" s="10"/>
+      <c r="F226" s="10"/>
+    </row>
+    <row r="227" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A227" s="8" t="s">
         <v>235</v>
       </c>
@@ -6713,8 +6738,15 @@
         <f>COUNT(Poblacion[Hombres])</f>
         <v>223</v>
       </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D227" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="F227" s="9">
+        <f>MAX(Poblacion[Mujeres])-MIN(Poblacion[Mujeres])</f>
+        <v>618474</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="8" t="s">
         <v>236</v>
       </c>
@@ -6722,8 +6754,15 @@
         <f>SUM(Poblacion[Hombres])</f>
         <v>3014881</v>
       </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D228" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="F228" s="9">
+        <f>QUARTILE(Poblacion[Mujeres],3)-QUARTILE(Poblacion[Mujeres],1)</f>
+        <v>7583.5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="8" t="s">
         <v>237</v>
       </c>
@@ -6731,8 +6770,15 @@
         <f>B228/B227</f>
         <v>13519.645739910315</v>
       </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D229" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="F229" s="9">
+        <f>_xlfn.VAR.P(Poblacion[Mujeres])</f>
+        <v>2961608666.7171268</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="8" t="s">
         <v>238</v>
       </c>
@@ -6740,8 +6786,15 @@
         <f>AVERAGE(Poblacion[Hombres])</f>
         <v>13519.645739910315</v>
       </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D230" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="F230" s="9">
+        <f>_xlfn.STDEV.P(Poblacion[Mujeres])</f>
+        <v>54420.663967992223</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="8" t="s">
         <v>239</v>
       </c>
@@ -6749,8 +6802,15 @@
         <f>TRIMMEAN(Poblacion[Hombres], 0.2)</f>
         <v>4355.1340782122907</v>
       </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D231" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="F231" s="9">
+        <f>STDEVP(Poblacion[Mujeres])/AVERAGE(Poblacion[Mujeres])</f>
+        <v>4.0834276249668617</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="8" t="s">
         <v>240</v>
       </c>
@@ -6759,7 +6819,7 @@
         <v>2536.2699728417242</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="8" t="s">
         <v>242</v>
       </c>
@@ -6768,7 +6828,7 @@
         <v>63.023467423566082</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="8" t="s">
         <v>243</v>
       </c>
@@ -6777,7 +6837,7 @@
         <v>4513</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="8" t="s">
         <v>244</v>
       </c>
@@ -6786,7 +6846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="8" t="s">
         <v>245</v>
       </c>
@@ -6799,8 +6859,9 @@
   <sortState ref="A2:F224">
     <sortCondition ref="B17"/>
   </sortState>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A226:B226"/>
+    <mergeCell ref="D226:F226"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Hoja con medidas de forma
</commit_message>
<xml_diff>
--- a/04/PoblacionMundial.xlsx
+++ b/04/PoblacionMundial.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="257">
   <si>
     <t>Continente</t>
   </si>
@@ -829,14 +829,30 @@
   </si>
   <si>
     <t>Coef. Var. Pearson</t>
+  </si>
+  <si>
+    <t>Medidas de forma</t>
+  </si>
+  <si>
+    <t>Coef. Asim. Pearson</t>
+  </si>
+  <si>
+    <t>Coef. Bowley</t>
+  </si>
+  <si>
+    <t>Coef. Fisher</t>
+  </si>
+  <si>
+    <t>Curtosis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -912,7 +928,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -938,6 +954,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Encabezado 1" xfId="2" builtinId="16"/>
@@ -1329,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G236"/>
+  <dimension ref="A1:J236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
-      <selection activeCell="F231" sqref="F231"/>
+    <sheetView tabSelected="1" topLeftCell="C224" workbookViewId="0">
+      <selection activeCell="J230" sqref="J230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,6 +1359,7 @@
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -6719,7 +6737,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="226" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A226" s="10" t="s">
         <v>241</v>
       </c>
@@ -6729,8 +6747,13 @@
       </c>
       <c r="E226" s="10"/>
       <c r="F226" s="10"/>
-    </row>
-    <row r="227" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H226" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="I226" s="10"/>
+      <c r="J226" s="10"/>
+    </row>
+    <row r="227" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A227" s="8" t="s">
         <v>235</v>
       </c>
@@ -6745,8 +6768,15 @@
         <f>MAX(Poblacion[Mujeres])-MIN(Poblacion[Mujeres])</f>
         <v>618474</v>
       </c>
-    </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H227" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="J227" s="11">
+        <f>(AVERAGE(Poblacion[Total])-MODE(Poblacion[Total]))/_xlfn.STDEV.P(Poblacion[Total])</f>
+        <v>0.23998237365523298</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="8" t="s">
         <v>236</v>
       </c>
@@ -6761,8 +6791,15 @@
         <f>QUARTILE(Poblacion[Mujeres],3)-QUARTILE(Poblacion[Mujeres],1)</f>
         <v>7583.5</v>
       </c>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H228" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="J228" s="11">
+        <f>(QUARTILE(Poblacion[Total],3)+QUARTILE(Poblacion[Total],1)-2*MEDIAN(Poblacion[Total]))/(QUARTILE(Poblacion[Total],3)-QUARTILE(Poblacion[Total],1))</f>
+        <v>0.46130295947591926</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="8" t="s">
         <v>237</v>
       </c>
@@ -6777,8 +6814,15 @@
         <f>_xlfn.VAR.P(Poblacion[Mujeres])</f>
         <v>2961608666.7171268</v>
       </c>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H229" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="J229" s="11">
+        <f>SKEW(Poblacion[Total])</f>
+        <v>9.308138992992891</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="8" t="s">
         <v>238</v>
       </c>
@@ -6793,8 +6837,15 @@
         <f>_xlfn.STDEV.P(Poblacion[Mujeres])</f>
         <v>54420.663967992223</v>
       </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H230" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="J230" s="11">
+        <f>KURT(Poblacion[Total])</f>
+        <v>94.087876378324253</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="8" t="s">
         <v>239</v>
       </c>
@@ -6810,7 +6861,7 @@
         <v>4.0834276249668617</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="8" t="s">
         <v>240</v>
       </c>
@@ -6819,7 +6870,7 @@
         <v>2536.2699728417242</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="8" t="s">
         <v>242</v>
       </c>
@@ -6828,7 +6879,7 @@
         <v>63.023467423566082</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="8" t="s">
         <v>243</v>
       </c>
@@ -6837,7 +6888,7 @@
         <v>4513</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="8" t="s">
         <v>244</v>
       </c>
@@ -6846,7 +6897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="8" t="s">
         <v>245</v>
       </c>
@@ -6859,9 +6910,10 @@
   <sortState ref="A2:F224">
     <sortCondition ref="B17"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A226:B226"/>
     <mergeCell ref="D226:F226"/>
+    <mergeCell ref="H226:J226"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>